<commit_message>
Arbeiten an Dokumentation (*)
Kapitel "Realisierung" fortgesetzt.
Einige Bilder nachgetragen.

* Color-Picker der Schicht-Bearbeitung gewechselt.
</commit_message>
<xml_diff>
--- a/docs/Zeitplan.xlsx
+++ b/docs/Zeitplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mail\Code\pelan\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CA6637-DCBB-489E-ACD3-2BAC5D86CEDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0DFC1B-5590-4400-B767-55A05870C988}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41235" yWindow="6060" windowWidth="20355" windowHeight="12765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="57">
   <si>
     <t>Zeitplan</t>
   </si>
@@ -1315,79 +1315,79 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1716,7 +1716,7 @@
   <dimension ref="B2:AS55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BB40" sqref="BB40"/>
+      <selection activeCell="AH33" sqref="AH33:AI33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1733,198 +1733,198 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:45" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="130" t="s">
+      <c r="B2" s="138" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
-      <c r="E2" s="131"/>
-      <c r="F2" s="131"/>
-      <c r="G2" s="131"/>
-      <c r="H2" s="131"/>
-      <c r="I2" s="131"/>
-      <c r="J2" s="131"/>
-      <c r="K2" s="131"/>
-      <c r="L2" s="131"/>
-      <c r="M2" s="131"/>
-      <c r="N2" s="131"/>
-      <c r="O2" s="131"/>
-      <c r="P2" s="131"/>
-      <c r="Q2" s="131"/>
-      <c r="R2" s="131"/>
-      <c r="S2" s="131"/>
-      <c r="T2" s="131"/>
-      <c r="U2" s="131"/>
-      <c r="V2" s="131"/>
-      <c r="W2" s="131"/>
-      <c r="X2" s="131"/>
-      <c r="Y2" s="131"/>
-      <c r="Z2" s="131"/>
-      <c r="AA2" s="131"/>
-      <c r="AB2" s="131"/>
-      <c r="AC2" s="131"/>
-      <c r="AD2" s="131"/>
-      <c r="AE2" s="131"/>
-      <c r="AF2" s="131"/>
-      <c r="AG2" s="131"/>
-      <c r="AH2" s="131"/>
-      <c r="AI2" s="131"/>
-      <c r="AJ2" s="131"/>
-      <c r="AK2" s="131"/>
-      <c r="AL2" s="131"/>
-      <c r="AM2" s="131"/>
-      <c r="AN2" s="131"/>
-      <c r="AO2" s="131"/>
-      <c r="AP2" s="131"/>
-      <c r="AQ2" s="131"/>
-      <c r="AR2" s="131"/>
-      <c r="AS2" s="132"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
+      <c r="E2" s="139"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="139"/>
+      <c r="H2" s="139"/>
+      <c r="I2" s="139"/>
+      <c r="J2" s="139"/>
+      <c r="K2" s="139"/>
+      <c r="L2" s="139"/>
+      <c r="M2" s="139"/>
+      <c r="N2" s="139"/>
+      <c r="O2" s="139"/>
+      <c r="P2" s="139"/>
+      <c r="Q2" s="139"/>
+      <c r="R2" s="139"/>
+      <c r="S2" s="139"/>
+      <c r="T2" s="139"/>
+      <c r="U2" s="139"/>
+      <c r="V2" s="139"/>
+      <c r="W2" s="139"/>
+      <c r="X2" s="139"/>
+      <c r="Y2" s="139"/>
+      <c r="Z2" s="139"/>
+      <c r="AA2" s="139"/>
+      <c r="AB2" s="139"/>
+      <c r="AC2" s="139"/>
+      <c r="AD2" s="139"/>
+      <c r="AE2" s="139"/>
+      <c r="AF2" s="139"/>
+      <c r="AG2" s="139"/>
+      <c r="AH2" s="139"/>
+      <c r="AI2" s="139"/>
+      <c r="AJ2" s="139"/>
+      <c r="AK2" s="139"/>
+      <c r="AL2" s="139"/>
+      <c r="AM2" s="139"/>
+      <c r="AN2" s="139"/>
+      <c r="AO2" s="139"/>
+      <c r="AP2" s="139"/>
+      <c r="AQ2" s="139"/>
+      <c r="AR2" s="139"/>
+      <c r="AS2" s="140"/>
     </row>
     <row r="3" spans="2:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="141" t="s">
+      <c r="B3" s="135" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="142"/>
-      <c r="D3" s="133" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="135"/>
-      <c r="F3" s="133" t="s">
+      <c r="C3" s="136"/>
+      <c r="D3" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="129"/>
+      <c r="F3" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="135"/>
-      <c r="J3" s="133" t="s">
+      <c r="G3" s="128"/>
+      <c r="H3" s="128"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="134"/>
-      <c r="L3" s="134"/>
-      <c r="M3" s="135"/>
-      <c r="N3" s="133" t="s">
+      <c r="K3" s="128"/>
+      <c r="L3" s="128"/>
+      <c r="M3" s="129"/>
+      <c r="N3" s="123" t="s">
         <v>36</v>
       </c>
-      <c r="O3" s="134"/>
-      <c r="P3" s="134"/>
-      <c r="Q3" s="135"/>
-      <c r="R3" s="133" t="s">
+      <c r="O3" s="128"/>
+      <c r="P3" s="128"/>
+      <c r="Q3" s="129"/>
+      <c r="R3" s="123" t="s">
         <v>37</v>
       </c>
-      <c r="S3" s="134"/>
-      <c r="T3" s="134"/>
-      <c r="U3" s="135"/>
-      <c r="V3" s="133" t="s">
+      <c r="S3" s="128"/>
+      <c r="T3" s="128"/>
+      <c r="U3" s="129"/>
+      <c r="V3" s="123" t="s">
         <v>38</v>
       </c>
-      <c r="W3" s="134"/>
-      <c r="X3" s="134"/>
-      <c r="Y3" s="135"/>
-      <c r="Z3" s="133" t="s">
+      <c r="W3" s="128"/>
+      <c r="X3" s="128"/>
+      <c r="Y3" s="129"/>
+      <c r="Z3" s="123" t="s">
         <v>39</v>
       </c>
-      <c r="AA3" s="134"/>
-      <c r="AB3" s="134"/>
-      <c r="AC3" s="135"/>
-      <c r="AD3" s="133" t="s">
+      <c r="AA3" s="128"/>
+      <c r="AB3" s="128"/>
+      <c r="AC3" s="129"/>
+      <c r="AD3" s="123" t="s">
         <v>40</v>
       </c>
-      <c r="AE3" s="134"/>
-      <c r="AF3" s="134"/>
-      <c r="AG3" s="135"/>
-      <c r="AH3" s="133" t="s">
+      <c r="AE3" s="128"/>
+      <c r="AF3" s="128"/>
+      <c r="AG3" s="129"/>
+      <c r="AH3" s="123" t="s">
         <v>41</v>
       </c>
-      <c r="AI3" s="134"/>
-      <c r="AJ3" s="134"/>
-      <c r="AK3" s="135"/>
-      <c r="AL3" s="133" t="s">
+      <c r="AI3" s="128"/>
+      <c r="AJ3" s="128"/>
+      <c r="AK3" s="129"/>
+      <c r="AL3" s="123" t="s">
         <v>42</v>
       </c>
-      <c r="AM3" s="134"/>
-      <c r="AN3" s="134"/>
-      <c r="AO3" s="135"/>
-      <c r="AP3" s="133" t="s">
+      <c r="AM3" s="128"/>
+      <c r="AN3" s="128"/>
+      <c r="AO3" s="129"/>
+      <c r="AP3" s="123" t="s">
         <v>43</v>
       </c>
-      <c r="AQ3" s="134"/>
-      <c r="AR3" s="134"/>
-      <c r="AS3" s="135"/>
+      <c r="AQ3" s="128"/>
+      <c r="AR3" s="128"/>
+      <c r="AS3" s="129"/>
     </row>
     <row r="4" spans="2:45" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="141"/>
-      <c r="C4" s="142"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="138"/>
-      <c r="F4" s="136" t="s">
+      <c r="B4" s="135"/>
+      <c r="C4" s="136"/>
+      <c r="D4" s="130"/>
+      <c r="E4" s="132"/>
+      <c r="F4" s="130" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="137"/>
-      <c r="H4" s="137"/>
-      <c r="I4" s="138"/>
-      <c r="J4" s="136" t="s">
+      <c r="G4" s="131"/>
+      <c r="H4" s="131"/>
+      <c r="I4" s="132"/>
+      <c r="J4" s="130" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="137"/>
-      <c r="L4" s="137"/>
-      <c r="M4" s="138"/>
-      <c r="N4" s="136" t="s">
+      <c r="K4" s="131"/>
+      <c r="L4" s="131"/>
+      <c r="M4" s="132"/>
+      <c r="N4" s="130" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="137"/>
-      <c r="P4" s="137"/>
-      <c r="Q4" s="138"/>
-      <c r="R4" s="136" t="s">
+      <c r="O4" s="131"/>
+      <c r="P4" s="131"/>
+      <c r="Q4" s="132"/>
+      <c r="R4" s="130" t="s">
         <v>28</v>
       </c>
-      <c r="S4" s="137"/>
-      <c r="T4" s="137"/>
-      <c r="U4" s="138"/>
-      <c r="V4" s="136" t="s">
+      <c r="S4" s="131"/>
+      <c r="T4" s="131"/>
+      <c r="U4" s="132"/>
+      <c r="V4" s="130" t="s">
         <v>29</v>
       </c>
-      <c r="W4" s="137"/>
-      <c r="X4" s="137"/>
-      <c r="Y4" s="138"/>
-      <c r="Z4" s="136" t="s">
+      <c r="W4" s="131"/>
+      <c r="X4" s="131"/>
+      <c r="Y4" s="132"/>
+      <c r="Z4" s="130" t="s">
         <v>30</v>
       </c>
-      <c r="AA4" s="137"/>
-      <c r="AB4" s="137"/>
-      <c r="AC4" s="138"/>
-      <c r="AD4" s="136" t="s">
+      <c r="AA4" s="131"/>
+      <c r="AB4" s="131"/>
+      <c r="AC4" s="132"/>
+      <c r="AD4" s="130" t="s">
         <v>31</v>
       </c>
-      <c r="AE4" s="137"/>
-      <c r="AF4" s="137"/>
-      <c r="AG4" s="138"/>
-      <c r="AH4" s="136" t="s">
+      <c r="AE4" s="131"/>
+      <c r="AF4" s="131"/>
+      <c r="AG4" s="132"/>
+      <c r="AH4" s="130" t="s">
         <v>32</v>
       </c>
-      <c r="AI4" s="137"/>
-      <c r="AJ4" s="137"/>
-      <c r="AK4" s="138"/>
-      <c r="AL4" s="136" t="s">
+      <c r="AI4" s="131"/>
+      <c r="AJ4" s="131"/>
+      <c r="AK4" s="132"/>
+      <c r="AL4" s="130" t="s">
         <v>33</v>
       </c>
-      <c r="AM4" s="137"/>
-      <c r="AN4" s="137"/>
-      <c r="AO4" s="138"/>
-      <c r="AP4" s="136" t="s">
+      <c r="AM4" s="131"/>
+      <c r="AN4" s="131"/>
+      <c r="AO4" s="132"/>
+      <c r="AP4" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="AQ4" s="137"/>
-      <c r="AR4" s="137"/>
-      <c r="AS4" s="138"/>
+      <c r="AQ4" s="131"/>
+      <c r="AR4" s="131"/>
+      <c r="AS4" s="132"/>
     </row>
     <row r="5" spans="2:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="139" t="s">
+      <c r="B5" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="140"/>
-      <c r="D5" s="143" t="s">
+      <c r="C5" s="134"/>
+      <c r="D5" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="140"/>
+      <c r="E5" s="134"/>
       <c r="F5" s="18">
         <v>2</v>
       </c>
@@ -2047,10 +2047,10 @@
       </c>
     </row>
     <row r="6" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="144" t="s">
+      <c r="B6" s="122" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="121" t="s">
+      <c r="C6" s="120" t="s">
         <v>47</v>
       </c>
       <c r="D6" s="112" t="s">
@@ -2101,8 +2101,8 @@
       <c r="AS6" s="12"/>
     </row>
     <row r="7" spans="2:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="133"/>
-      <c r="C7" s="121"/>
+      <c r="B7" s="123"/>
+      <c r="C7" s="120"/>
       <c r="D7" s="113" t="s">
         <v>8</v>
       </c>
@@ -2151,7 +2151,7 @@
       <c r="AS7" s="29"/>
     </row>
     <row r="8" spans="2:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="127" t="s">
+      <c r="B8" s="126" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="99"/>
@@ -2204,7 +2204,7 @@
       <c r="AS8" s="101"/>
     </row>
     <row r="9" spans="2:45" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="128"/>
+      <c r="B9" s="127"/>
       <c r="C9" s="103"/>
       <c r="D9" s="115" t="s">
         <v>8</v>
@@ -2255,10 +2255,10 @@
       <c r="AS9" s="104"/>
     </row>
     <row r="10" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="122" t="s">
+      <c r="B10" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="121" t="s">
+      <c r="C10" s="120" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="113" t="s">
@@ -2309,8 +2309,8 @@
       <c r="AS10" s="16"/>
     </row>
     <row r="11" spans="2:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="122"/>
-      <c r="C11" s="121"/>
+      <c r="B11" s="124"/>
+      <c r="C11" s="120"/>
       <c r="D11" s="116" t="s">
         <v>8</v>
       </c>
@@ -2359,8 +2359,8 @@
       <c r="AS11" s="43"/>
     </row>
     <row r="12" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="122"/>
-      <c r="C12" s="121" t="s">
+      <c r="B12" s="124"/>
+      <c r="C12" s="120" t="s">
         <v>46</v>
       </c>
       <c r="D12" s="113" t="s">
@@ -2411,8 +2411,8 @@
       <c r="AS12" s="16"/>
     </row>
     <row r="13" spans="2:45" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="122"/>
-      <c r="C13" s="121"/>
+      <c r="B13" s="124"/>
+      <c r="C13" s="120"/>
       <c r="D13" s="116" t="s">
         <v>8</v>
       </c>
@@ -2461,8 +2461,8 @@
       <c r="AS13" s="43"/>
     </row>
     <row r="14" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="122"/>
-      <c r="C14" s="121" t="s">
+      <c r="B14" s="124"/>
+      <c r="C14" s="120" t="s">
         <v>45</v>
       </c>
       <c r="D14" s="113" t="s">
@@ -2513,8 +2513,8 @@
       <c r="AS14" s="16"/>
     </row>
     <row r="15" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="126"/>
-      <c r="C15" s="124"/>
+      <c r="B15" s="125"/>
+      <c r="C15" s="121"/>
       <c r="D15" s="117" t="s">
         <v>8</v>
       </c>
@@ -2563,10 +2563,10 @@
       <c r="AS15" s="13"/>
     </row>
     <row r="16" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="125" t="s">
+      <c r="B16" s="142" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="123" t="s">
+      <c r="C16" s="143" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="112" t="s">
@@ -2617,8 +2617,8 @@
       <c r="AS16" s="16"/>
     </row>
     <row r="17" spans="2:45" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="122"/>
-      <c r="C17" s="121"/>
+      <c r="B17" s="124"/>
+      <c r="C17" s="120"/>
       <c r="D17" s="116" t="s">
         <v>8</v>
       </c>
@@ -2667,8 +2667,8 @@
       <c r="AS17" s="43"/>
     </row>
     <row r="18" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="122"/>
-      <c r="C18" s="121" t="s">
+      <c r="B18" s="124"/>
+      <c r="C18" s="120" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="113" t="s">
@@ -2719,8 +2719,8 @@
       <c r="AS18" s="16"/>
     </row>
     <row r="19" spans="2:45" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="122"/>
-      <c r="C19" s="121"/>
+      <c r="B19" s="124"/>
+      <c r="C19" s="120"/>
       <c r="D19" s="116" t="s">
         <v>8</v>
       </c>
@@ -2769,8 +2769,8 @@
       <c r="AS19" s="43"/>
     </row>
     <row r="20" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="122"/>
-      <c r="C20" s="121" t="s">
+      <c r="B20" s="124"/>
+      <c r="C20" s="120" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="113" t="s">
@@ -2821,8 +2821,8 @@
       <c r="AS20" s="16"/>
     </row>
     <row r="21" spans="2:45" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="122"/>
-      <c r="C21" s="121"/>
+      <c r="B21" s="124"/>
+      <c r="C21" s="120"/>
       <c r="D21" s="116" t="s">
         <v>8</v>
       </c>
@@ -2871,8 +2871,8 @@
       <c r="AS21" s="43"/>
     </row>
     <row r="22" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="122"/>
-      <c r="C22" s="121" t="s">
+      <c r="B22" s="124"/>
+      <c r="C22" s="120" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="113" t="s">
@@ -2923,8 +2923,8 @@
       <c r="AS22" s="16"/>
     </row>
     <row r="23" spans="2:45" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="122"/>
-      <c r="C23" s="121"/>
+      <c r="B23" s="124"/>
+      <c r="C23" s="120"/>
       <c r="D23" s="116" t="s">
         <v>8</v>
       </c>
@@ -2973,8 +2973,8 @@
       <c r="AS23" s="43"/>
     </row>
     <row r="24" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="122"/>
-      <c r="C24" s="121" t="s">
+      <c r="B24" s="124"/>
+      <c r="C24" s="120" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="113" t="s">
@@ -3025,8 +3025,8 @@
       <c r="AS24" s="16"/>
     </row>
     <row r="25" spans="2:45" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="122"/>
-      <c r="C25" s="121"/>
+      <c r="B25" s="124"/>
+      <c r="C25" s="120"/>
       <c r="D25" s="116" t="s">
         <v>8</v>
       </c>
@@ -3075,8 +3075,8 @@
       <c r="AS25" s="43"/>
     </row>
     <row r="26" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="122"/>
-      <c r="C26" s="121" t="s">
+      <c r="B26" s="124"/>
+      <c r="C26" s="120" t="s">
         <v>15</v>
       </c>
       <c r="D26" s="113" t="s">
@@ -3127,8 +3127,8 @@
       <c r="AS26" s="16"/>
     </row>
     <row r="27" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="126"/>
-      <c r="C27" s="124"/>
+      <c r="B27" s="125"/>
+      <c r="C27" s="121"/>
       <c r="D27" s="117" t="s">
         <v>8</v>
       </c>
@@ -3177,10 +3177,10 @@
       <c r="AS27" s="13"/>
     </row>
     <row r="28" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="122" t="s">
+      <c r="B28" s="124" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="121" t="s">
+      <c r="C28" s="120" t="s">
         <v>50</v>
       </c>
       <c r="D28" s="113" t="s">
@@ -3231,8 +3231,8 @@
       <c r="AS28" s="16"/>
     </row>
     <row r="29" spans="2:45" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="122"/>
-      <c r="C29" s="121"/>
+      <c r="B29" s="124"/>
+      <c r="C29" s="120"/>
       <c r="D29" s="116" t="s">
         <v>8</v>
       </c>
@@ -3281,8 +3281,8 @@
       <c r="AS29" s="43"/>
     </row>
     <row r="30" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="122"/>
-      <c r="C30" s="121" t="s">
+      <c r="B30" s="124"/>
+      <c r="C30" s="120" t="s">
         <v>51</v>
       </c>
       <c r="D30" s="113" t="s">
@@ -3333,8 +3333,8 @@
       <c r="AS30" s="16"/>
     </row>
     <row r="31" spans="2:45" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="122"/>
-      <c r="C31" s="121"/>
+      <c r="B31" s="124"/>
+      <c r="C31" s="120"/>
       <c r="D31" s="113" t="s">
         <v>8</v>
       </c>
@@ -3383,7 +3383,7 @@
       <c r="AS31" s="29"/>
     </row>
     <row r="32" spans="2:45" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="127" t="s">
+      <c r="B32" s="126" t="s">
         <v>11</v>
       </c>
       <c r="C32" s="99"/>
@@ -3433,10 +3433,10 @@
       <c r="AP32" s="119"/>
       <c r="AQ32" s="119"/>
       <c r="AR32" s="119"/>
-      <c r="AS32" s="120"/>
+      <c r="AS32" s="144"/>
     </row>
     <row r="33" spans="2:45" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="128"/>
+      <c r="B33" s="127"/>
       <c r="C33" s="103"/>
       <c r="D33" s="115" t="s">
         <v>8</v>
@@ -3473,8 +3473,8 @@
       <c r="AE33" s="102"/>
       <c r="AF33" s="102"/>
       <c r="AG33" s="102"/>
-      <c r="AH33" s="103"/>
-      <c r="AI33" s="103"/>
+      <c r="AH33" s="102"/>
+      <c r="AI33" s="102"/>
       <c r="AJ33" s="103"/>
       <c r="AK33" s="103"/>
       <c r="AL33" s="103"/>
@@ -3487,10 +3487,10 @@
       <c r="AS33" s="104"/>
     </row>
     <row r="34" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="122" t="s">
+      <c r="B34" s="124" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="121" t="s">
+      <c r="C34" s="120" t="s">
         <v>55</v>
       </c>
       <c r="D34" s="113" t="s">
@@ -3541,8 +3541,8 @@
       <c r="AS34" s="16"/>
     </row>
     <row r="35" spans="2:45" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="122"/>
-      <c r="C35" s="121"/>
+      <c r="B35" s="124"/>
+      <c r="C35" s="120"/>
       <c r="D35" s="116" t="s">
         <v>8</v>
       </c>
@@ -3591,8 +3591,8 @@
       <c r="AS35" s="43"/>
     </row>
     <row r="36" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="122"/>
-      <c r="C36" s="129" t="s">
+      <c r="B36" s="124"/>
+      <c r="C36" s="141" t="s">
         <v>48</v>
       </c>
       <c r="D36" s="113" t="s">
@@ -3643,8 +3643,8 @@
       <c r="AS36" s="16"/>
     </row>
     <row r="37" spans="2:45" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="122"/>
-      <c r="C37" s="129"/>
+      <c r="B37" s="124"/>
+      <c r="C37" s="141"/>
       <c r="D37" s="116" t="s">
         <v>8</v>
       </c>
@@ -3693,8 +3693,8 @@
       <c r="AS37" s="43"/>
     </row>
     <row r="38" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="122"/>
-      <c r="C38" s="121" t="s">
+      <c r="B38" s="124"/>
+      <c r="C38" s="120" t="s">
         <v>56</v>
       </c>
       <c r="D38" s="113" t="s">
@@ -3745,8 +3745,8 @@
       <c r="AS38" s="16"/>
     </row>
     <row r="39" spans="2:45" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="122"/>
-      <c r="C39" s="121"/>
+      <c r="B39" s="124"/>
+      <c r="C39" s="120"/>
       <c r="D39" s="116" t="s">
         <v>8</v>
       </c>
@@ -3795,8 +3795,8 @@
       <c r="AS39" s="43"/>
     </row>
     <row r="40" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="122"/>
-      <c r="C40" s="121" t="s">
+      <c r="B40" s="124"/>
+      <c r="C40" s="120" t="s">
         <v>20</v>
       </c>
       <c r="D40" s="113" t="s">
@@ -3847,8 +3847,8 @@
       <c r="AS40" s="16"/>
     </row>
     <row r="41" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="126"/>
-      <c r="C41" s="124"/>
+      <c r="B41" s="125"/>
+      <c r="C41" s="121"/>
       <c r="D41" s="117" t="s">
         <v>8</v>
       </c>
@@ -3897,10 +3897,10 @@
       <c r="AS41" s="13"/>
     </row>
     <row r="42" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="125" t="s">
+      <c r="B42" s="142" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="123" t="s">
+      <c r="C42" s="143" t="s">
         <v>22</v>
       </c>
       <c r="D42" s="112" t="s">
@@ -3951,8 +3951,8 @@
       <c r="AS42" s="11"/>
     </row>
     <row r="43" spans="2:45" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="122"/>
-      <c r="C43" s="121"/>
+      <c r="B43" s="124"/>
+      <c r="C43" s="120"/>
       <c r="D43" s="116" t="s">
         <v>8</v>
       </c>
@@ -4001,8 +4001,8 @@
       <c r="AS43" s="43"/>
     </row>
     <row r="44" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="122"/>
-      <c r="C44" s="121" t="s">
+      <c r="B44" s="124"/>
+      <c r="C44" s="120" t="s">
         <v>23</v>
       </c>
       <c r="D44" s="113" t="s">
@@ -4053,8 +4053,8 @@
       <c r="AS44" s="21"/>
     </row>
     <row r="45" spans="2:45" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="122"/>
-      <c r="C45" s="121"/>
+      <c r="B45" s="124"/>
+      <c r="C45" s="120"/>
       <c r="D45" s="116" t="s">
         <v>8</v>
       </c>
@@ -4087,8 +4087,8 @@
       <c r="AE45" s="45"/>
       <c r="AF45" s="44"/>
       <c r="AG45" s="75"/>
-      <c r="AH45" s="57"/>
-      <c r="AI45" s="42"/>
+      <c r="AH45" s="61"/>
+      <c r="AI45" s="44"/>
       <c r="AJ45" s="42"/>
       <c r="AK45" s="71"/>
       <c r="AL45" s="82"/>
@@ -4101,8 +4101,8 @@
       <c r="AS45" s="46"/>
     </row>
     <row r="46" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="122"/>
-      <c r="C46" s="121" t="s">
+      <c r="B46" s="124"/>
+      <c r="C46" s="120" t="s">
         <v>49</v>
       </c>
       <c r="D46" s="113" t="s">
@@ -4153,8 +4153,8 @@
       <c r="AS46" s="21"/>
     </row>
     <row r="47" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="126"/>
-      <c r="C47" s="124"/>
+      <c r="B47" s="125"/>
+      <c r="C47" s="121"/>
       <c r="D47" s="117" t="s">
         <v>8</v>
       </c>
@@ -4201,10 +4201,10 @@
       <c r="AS47" s="35"/>
     </row>
     <row r="48" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="122" t="s">
+      <c r="B48" s="124" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="123" t="s">
+      <c r="C48" s="143" t="s">
         <v>54</v>
       </c>
       <c r="D48" s="112" t="s">
@@ -4255,8 +4255,8 @@
       <c r="AS48" s="37"/>
     </row>
     <row r="49" spans="2:45" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="122"/>
-      <c r="C49" s="121"/>
+      <c r="B49" s="124"/>
+      <c r="C49" s="120"/>
       <c r="D49" s="116" t="s">
         <v>8</v>
       </c>
@@ -4303,8 +4303,8 @@
       <c r="AS49" s="46"/>
     </row>
     <row r="50" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="122"/>
-      <c r="C50" s="121" t="s">
+      <c r="B50" s="124"/>
+      <c r="C50" s="120" t="s">
         <v>19</v>
       </c>
       <c r="D50" s="113" t="s">
@@ -4355,8 +4355,8 @@
       <c r="AS50" s="37"/>
     </row>
     <row r="51" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="126"/>
-      <c r="C51" s="124"/>
+      <c r="B51" s="125"/>
+      <c r="C51" s="121"/>
       <c r="D51" s="118" t="s">
         <v>8</v>
       </c>
@@ -4403,10 +4403,10 @@
       <c r="AS51" s="35"/>
     </row>
     <row r="52" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="125" t="s">
+      <c r="B52" s="142" t="s">
         <v>18</v>
       </c>
-      <c r="C52" s="123" t="s">
+      <c r="C52" s="143" t="s">
         <v>24</v>
       </c>
       <c r="D52" s="112" t="s">
@@ -4457,8 +4457,8 @@
       <c r="AS52" s="21"/>
     </row>
     <row r="53" spans="2:45" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="122"/>
-      <c r="C53" s="121"/>
+      <c r="B53" s="124"/>
+      <c r="C53" s="120"/>
       <c r="D53" s="116" t="s">
         <v>8</v>
       </c>
@@ -4505,8 +4505,8 @@
       <c r="AS53" s="46"/>
     </row>
     <row r="54" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="122"/>
-      <c r="C54" s="121" t="s">
+      <c r="B54" s="124"/>
+      <c r="C54" s="120" t="s">
         <v>20</v>
       </c>
       <c r="D54" s="113" t="s">
@@ -4557,8 +4557,8 @@
       <c r="AS54" s="39"/>
     </row>
     <row r="55" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="126"/>
-      <c r="C55" s="124"/>
+      <c r="B55" s="125"/>
+      <c r="C55" s="121"/>
       <c r="D55" s="117" t="s">
         <v>8</v>
       </c>
@@ -4606,23 +4606,33 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="F8:V8"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="D3:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="X32:AS32"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="B16:B27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="B34:B41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="B42:B47"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C50:C51"/>
     <mergeCell ref="B2:AS2"/>
     <mergeCell ref="AP3:AS3"/>
     <mergeCell ref="Z4:AC4"/>
@@ -4639,33 +4649,23 @@
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="B34:B41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="B42:B47"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="X32:AS32"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="B16:B27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="F8:V8"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="52" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>